<commit_message>
Ajuste arquivo de novas sentenças
</commit_message>
<xml_diff>
--- a/new_sentences/newSentences.xlsx
+++ b/new_sentences/newSentences.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\INSPER\Engenharia\7-Semestre\PLN\Chatbot\new_sentences\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63BB4D7-0C27-412F-ADCC-21020D61CE7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2166" yWindow="2166" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Sentença</t>
   </si>
@@ -22,45 +28,12 @@
     <t>Intenção</t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>Hoje tem gol do Gabigol?</t>
   </si>
   <si>
-    <t>Qual a mínima de hoje?</t>
-  </si>
-  <si>
-    <t>Vai nevar no sábado?</t>
-  </si>
-  <si>
-    <t>Acender a luz, por favor!</t>
-  </si>
-  <si>
-    <t>luz</t>
-  </si>
-  <si>
-    <t>Ligue a luz, por favor!</t>
-  </si>
-  <si>
-    <t>foxbot, mostra a minha conta bancaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mostra minha conta aí foxbot! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salve foxbot! Mostra meu saldo, por favor. </t>
-  </si>
-  <si>
     <t>O Thiago tem pipi grande?</t>
   </si>
   <si>
-    <t xml:space="preserve">Qual a previsão do tempo pra domingo? </t>
-  </si>
-  <si>
-    <t>mostra a minha conta bancaria, foxbot</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mostre uma imagem do meu Ma </t>
   </si>
   <si>
@@ -70,12 +43,6 @@
     <t xml:space="preserve">Quanto foi o jogo do Palmeiras hoje? </t>
   </si>
   <si>
-    <t xml:space="preserve">Quantos graus tá agora? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ligue o ar condicionado imediatamente </t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantas estrelas existem no céu? </t>
   </si>
   <si>
@@ -100,16 +67,16 @@
     <t xml:space="preserve">dinheiro </t>
   </si>
   <si>
-    <t>Consultar saldo da conta</t>
+    <t xml:space="preserve">Como tô de dinheiro? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vai chover hoje? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liga a luz aí </t>
   </si>
   <si>
     <t>Não sei</t>
-  </si>
-  <si>
-    <t>Obter informações relativas ao clima</t>
-  </si>
-  <si>
-    <t>Interagir com a luz ou o ar-condicionado</t>
   </si>
   <si>
     <t>Temperatura</t>
@@ -133,8 +100,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +164,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +250,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +302,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,14 +495,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -507,10 +520,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -518,10 +531,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -529,10 +542,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -540,10 +553,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -551,10 +564,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -562,10 +575,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -573,10 +586,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -584,10 +597,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -595,10 +608,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -606,10 +619,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -617,10 +630,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -628,10 +641,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -639,10 +652,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -650,10 +663,10 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -661,10 +674,10 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -672,117 +685,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
         <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>